<commit_message>
This is third changes in master
</commit_message>
<xml_diff>
--- a/Data/ExternalFileForSelinum.xlsx
+++ b/Data/ExternalFileForSelinum.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\software_Testing\Selinum\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20055" windowHeight="7695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="5175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L15"/>
 </workbook>
 </file>
 

</xml_diff>